<commit_message>
Casos de teste de 5 até 10
</commit_message>
<xml_diff>
--- a/documentation/Casos de Teste.xlsx
+++ b/documentation/Casos de Teste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="UC.01" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="170">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -288,10 +288,6 @@
   </si>
   <si>
     <t>Não executado</t>
-  </si>
-  <si>
-    <t>O Sistema mostra a Janela para criar thread
-Sistema mostra aviso de envio bem sucedido</t>
   </si>
   <si>
     <t>5. Sistema adiciona a thread criada ao grupo de threads ativas nas tags selecionada</t>
@@ -1106,6 +1102,501 @@
       </rPr>
       <t>thread em destaque</t>
     </r>
+  </si>
+  <si>
+    <t>1. Usuário seleciona o botão Opções no cabeçalho do sistema ou o ícone Alterar CSS existente no perfil de usuário</t>
+  </si>
+  <si>
+    <t>2. Sistema exibe um modal com campo de texto para inserir o código CSS</t>
+  </si>
+  <si>
+    <t>5. Sistema adiciona o CSS inserido às páginas do sistema</t>
+  </si>
+  <si>
+    <t>4. Usuário seleciona o botão Save</t>
+  </si>
+  <si>
+    <t>3. Usuário preenche o campo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no botão opções
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> body{
+  color: ed4845;
+font-size: 32px;
+}
+Clicar no botão Save</t>
+    </r>
+  </si>
+  <si>
+    <t>Usuário observa fontes vermelhas e de Tamanho 32px por todo texto do site</t>
+  </si>
+  <si>
+    <t>Usuário insere um CSS inválido</t>
+  </si>
+  <si>
+    <t>Sistema exibe uma mensagem de erro e permanece na janela de preenchimento do código CSS</t>
+  </si>
+  <si>
+    <t>Clicar no botão opções
+CSS: bodi{
+  color: ed4845;
+font-e: 32px;
+Clicar no botão Save</t>
+  </si>
+  <si>
+    <t>2. Sistema exibe um modal com campo de captcha</t>
+  </si>
+  <si>
+    <t>1. Usuário seleciona o ícone ao lado do id do post</t>
+  </si>
+  <si>
+    <t>3. Usuário soluciona o captcha</t>
+  </si>
+  <si>
+    <t>4. Usuário seleciona o botão Report</t>
+  </si>
+  <si>
+    <t>5. Sistema notifica os administradores e salva a denúncia na lista de denúncias</t>
+  </si>
+  <si>
+    <t>Sistema exibe uma janela para preencher os dados do post
+Sistema exibe uma mensagem de postagem bem sucedida e o comentário aparece na thread</t>
+  </si>
+  <si>
+    <t>O Sistema mostra a Janela para criar thread
+Sistema mostra aviso de envio bem sucedido e a thread fica visível na s tags especificadas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no ícone de report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Captcha:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> clicar no captcha
+Clicar no botão Report</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibe uma janela para solucionar o captcha
+Administradores recebem uma notificação e o comentário denunciado fica visível na lista de denúncias</t>
+  </si>
+  <si>
+    <t>Usuário não soluciona o captcha</t>
+  </si>
+  <si>
+    <t>Clicar no ícone de report
+Clicar no botão Report</t>
+  </si>
+  <si>
+    <t>Sistema mostra aviso de que o captcha não foi completado e permanece na janela de denúncia</t>
+  </si>
+  <si>
+    <t>1. Usuário seleciona o botão Sign Up no cabeçalho do sistema</t>
+  </si>
+  <si>
+    <t>2. Sistema exibe um modal com os seguintes campos para serem preenchidos: Login, Password, e-mail e área para realizar o upload de imagem de perfil</t>
+  </si>
+  <si>
+    <t>3. Usuário preenche os campos e opcionalmente escolhe e realiza o upload da imagem de perfil</t>
+  </si>
+  <si>
+    <t>4. Usuário seleciona o botão Enter</t>
+  </si>
+  <si>
+    <t>5. Sistema valida os campos preenchidos e efetua o cadastro</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no botão Sign Up
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Teste
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 123456
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e-mail: Teste@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Upload:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> imgPerfil.png
+Clicar no botão Enter</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibe janela para preenchimento do cadastro
+Sistema exibe mensagem de sucesso, cria a conta e envia e-mail de confirmação</t>
+  </si>
+  <si>
+    <t>Usuário coloca um e-mail inválido</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no botão Sign Up
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Teste
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 123456
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Testegmail.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Upload:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> imgPerfil.png
+Clicar no botão Enter</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibe mensagem de falha no e-mail e permanece na janela de cadastro</t>
+  </si>
+  <si>
+    <t>Usuário não preenche o campo de login</t>
+  </si>
+  <si>
+    <t>Clicar no botão Sign Up
+Password: 123456
+e-mail: Testegmail.com
+Upload: imgPerfil.png
+Clicar no botão Enter</t>
+  </si>
+  <si>
+    <t>Sistema exibe mensagem de que faltou o preenchimento do login e permanece na janela de cadastro</t>
+  </si>
+  <si>
+    <t>Usuário não preenche o campo de password</t>
+  </si>
+  <si>
+    <t>Clicar no botão Sign Up
+Login: Teste
+e-mail: Testegmail.com
+Upload: imgPerfil.png
+Clicar no botão Enter</t>
+  </si>
+  <si>
+    <t>Sistema exibe mensagem de que faltou o preenchimento do password e permanece na janela de cadastro</t>
+  </si>
+  <si>
+    <t>1. Usuário cadastrado clica em seu nome de usuário no cabeçalho do sistema para acessar seu perfil</t>
+  </si>
+  <si>
+    <t>2. Sistema exibe a pagina de perfil</t>
+  </si>
+  <si>
+    <t>3. Usuário aperta o ícone de alteração de configurações</t>
+  </si>
+  <si>
+    <t>4. Sistema exibe uma tela para alteração de configurações, incluindo alteração de senha e nome de usuário.</t>
+  </si>
+  <si>
+    <t>5. Usuário preenche os campos que deseja alterar</t>
+  </si>
+  <si>
+    <t>6. Usuário clica no botão alterar</t>
+  </si>
+  <si>
+    <t>7. Sistema valida as alterações realizadas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no próprio nome de usuário
+Clicar no ícone de alteração de configurações
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Novo nome de usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Teste2
+Clicar no botão alterar</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibe página de perfil
+Sistema exibe página para alteração de configurações
+Sistema exibe mensagem de sucesso e altera o nome de usuário para Teste2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no próprio nome de usuário
+Clicar no ícone de alteração de configurações
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nova senha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 654321
+Clicar no botão alterar</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibe página de perfil
+Sistema exibe página para alteração de configurações
+Sistema exibe mensagem de sucesso e altera a senha do usuário para 654321</t>
+  </si>
+  <si>
+    <t>1. Usuário cadastrado localiza a thread que deseja marcar</t>
+  </si>
+  <si>
+    <t>2. Usuário cadastrado aperta no ícone de Marcar para Visualização na postagem inicial da thread</t>
+  </si>
+  <si>
+    <t>3. Sistema adiciona a thread na lista de threads visualizadas do usuário cadastrado</t>
+  </si>
+  <si>
+    <t>1. Usuário cria uma thread</t>
+  </si>
+  <si>
+    <t>2. Sistema adiciona a thread na lista de threads visualizadas do usuário cadastrado</t>
+  </si>
+  <si>
+    <t>Clicar no botão New Thread
+Subject: Titulo1
+Comment: Teste
+Tag: Anime e História
+Captcha: clicar no captcha
+Clicar no botão Post</t>
+  </si>
+  <si>
+    <t>Thread aparece na lista de threads visualizadas dentro do perfil do usuário cadastrado</t>
+  </si>
+  <si>
+    <t>3. Usuário cadastrado seleciona o ícone Gerenciar Notificações</t>
+  </si>
+  <si>
+    <t>4. Sistema exibe uma tela com opções de retirar threads marcadas de sua lista ou apenas silenciar o envio de notificações de determinada thread</t>
+  </si>
+  <si>
+    <t>5. Usuário cadastrado seleciona a thread da lista e a opção que deseja efetuar</t>
+  </si>
+  <si>
+    <t>6. Sistema salva a alteração realizada</t>
+  </si>
+  <si>
+    <t>Clicar na thread com subject: "Titulo1"
+Clicar no ícone de Marcar para Visualização</t>
+  </si>
+  <si>
+    <t>Clicar no próprio nome de usuário
+Clicar no ícone Gerenciar Notificações
+Selecionar a thread com subject "Titulo1" 
+Clicar na opção Silenciar Thread</t>
+  </si>
+  <si>
+    <t>Sistema exibe a página de perfil
+Sistema exibe a janela de Gerenciar Notificações
+Usuário para de receber notificações da thread "Titulo1", porém ela continua na lista de thread visualizadas</t>
+  </si>
+  <si>
+    <t>Clicar no próprio nome de usuário
+Clicar no ícone Gerenciar Notificações
+Selecionar a thread com subject "Titulo1" 
+Clicar na opção Retirar da Lista de Threads</t>
+  </si>
+  <si>
+    <t>Sistema exibe a página de perfil
+Sistema exibe a janela de Gerenciar Notificações
+Usuário para de receber notificações da thread "Titulo1" e ela é retirada da lista de threads para visualização</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1403,6 +1894,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1452,11 +1952,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="110">
     <dxf>
       <font>
         <color rgb="FF7030A0"/>
@@ -1954,6 +2457,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00B050"/>
       </font>
       <fill>
@@ -1965,6 +2483,61 @@
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
       </font>
     </dxf>
     <dxf>
@@ -2310,7 +2883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2334,11 +2907,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2376,12 +2949,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2404,110 +2977,110 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4" t="s">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2526,26 +3099,26 @@
     <mergeCell ref="F11:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F13">
-    <cfRule type="containsText" dxfId="97" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="103" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="102" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="100" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="99" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="92" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2556,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,16 +3150,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2611,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F128,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F128,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2624,12 +3197,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2651,92 +3224,189 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="37"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="D12:D17"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F30 F30:F1048576">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2767,16 +3437,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2814,12 +3484,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2842,58 +3512,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2907,26 +3577,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2957,16 +3627,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3004,12 +3674,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3032,58 +3702,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3097,26 +3767,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3147,16 +3817,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3194,12 +3864,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3222,58 +3892,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3287,26 +3957,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3337,16 +4007,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3384,12 +4054,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3412,58 +4082,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3477,26 +4147,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3527,16 +4197,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3574,12 +4244,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3602,58 +4272,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3667,26 +4337,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3717,16 +4387,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3764,12 +4434,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3792,58 +4462,58 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3857,26 +4527,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3888,8 +4558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,16 +4577,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3954,12 +4624,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3982,133 +4652,133 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="C6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+        <v>34</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+      <c r="A11" s="29">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="32" t="s">
+      <c r="C11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="33"/>
+        <v>34</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="34"/>
+        <v>28</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
@@ -4120,13 +4790,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="8" t="s">
@@ -4138,13 +4808,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="D18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
@@ -4155,11 +4825,11 @@
       <c r="A19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -4178,34 +4848,34 @@
     <mergeCell ref="F11:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="91" priority="13" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="97" priority="13" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="14" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="96" priority="14" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="11" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="94" priority="11" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="12" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F15">
-    <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="92" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="91" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4218,8 +4888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4237,16 +4907,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4284,12 +4954,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4312,133 +4982,133 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="29" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="D11" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4" t="s">
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18" t="s">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
-        <v>2</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="33"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="33"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>3</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="12" t="s">
@@ -4450,13 +5120,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12" t="s">
@@ -4464,75 +5134,86 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="29">
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="33"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="33"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="F18:F22"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A10"/>
@@ -4540,39 +5221,28 @@
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F11">
-    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="5" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="6" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="85" priority="6" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F18 F23:F1048576">
-    <cfRule type="cellIs" dxfId="78" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4584,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -4603,16 +5273,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4650,12 +5320,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4678,113 +5348,113 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>2</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="D10" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4" t="s">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
-        <v>2</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="29" t="s">
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="33"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>3</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="12" t="s">
@@ -4795,14 +5465,20 @@
       <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A9"/>
@@ -4810,34 +5486,28 @@
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="F6:F9"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="83" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="82" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F30 F30:F1048576">
-    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4847,10 +5517,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,16 +5538,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4902,7 +5572,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F122,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F122,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4915,12 +5585,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4942,63 +5612,95 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A10"/>
@@ -5007,40 +5709,41 @@
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F11">
+    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5058,16 +5761,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5092,7 +5795,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F122,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F122,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5105,12 +5808,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5132,63 +5835,95 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A10"/>
@@ -5197,27 +5932,27 @@
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F11">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5227,10 +5962,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5248,16 +5983,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5282,7 +6017,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F124,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F124,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5295,12 +6030,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5322,63 +6057,131 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A10"/>
@@ -5387,27 +6190,27 @@
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="59" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F13">
+    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5417,10 +6220,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5438,16 +6241,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5472,7 +6275,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F130,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F130,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5485,12 +6288,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5512,92 +6315,209 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="36"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="F13:F19"/>
+    <mergeCell ref="B20:F20"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="F6:F12"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="D13:D19"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6">
+    <cfRule type="containsText" dxfId="59" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="58" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F30 F30:F1048576">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5609,8 +6529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5628,16 +6548,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5675,12 +6595,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5702,92 +6622,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32" t="s">
+      <c r="B6" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
+      <c r="A9" s="29">
+        <v>2</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F9">
+    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F9 F11:F1048576">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Versão inicial dos casos de teste finalizados
</commit_message>
<xml_diff>
--- a/documentation/Casos de Teste.xlsx
+++ b/documentation/Casos de Teste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="UC.01" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="227">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -1598,12 +1598,245 @@
 Sistema exibe a janela de Gerenciar Notificações
 Usuário para de receber notificações da thread "Titulo1" e ela é retirada da lista de threads para visualização</t>
   </si>
+  <si>
+    <t>1. Sistema verifica que uma das threads na lista de threads para visualização do usuário cadastrado recebeu uma nova postagem</t>
+  </si>
+  <si>
+    <t>3. Usuário cadastrado verifica a notificação em seu cabeçalho, tendo a opção de deletar ou permitir que a notificação permaneça na lista de notificações</t>
+  </si>
+  <si>
+    <t>2. Sistema envia uma notificação para o cabeçalho do usuário cadastrado contendo a informação de qual thread recebeu uma nova postagem, a hora da postagem e um link para a postagem na thread</t>
+  </si>
+  <si>
+    <t>(Necessário ter a thread com subject "Teste3" na lista de threads visualizadas para receber a notificação)
+Realizar a postagem de um comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação
+Fechar a aba de notificações
+Reabrir a aba de notificações</t>
+  </si>
+  <si>
+    <t>(Necessário ter a thread com subject "Teste3" na lista de threads visualizadas para receber a notificação)
+Realizar a postagem de um comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação
+Clicar para deletar a notificação
+Reabrir a aba de notificações</t>
+  </si>
+  <si>
+    <t>No passo 2, caso já exista uma notificação da mesma thread na lista de notificações do usuário cadastrado, o sistema não envia a nova notificação</t>
+  </si>
+  <si>
+    <t>Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário
+Sistema marca notificação como visualizada
+Notificação permanece na aba de notificações do usuário</t>
+  </si>
+  <si>
+    <t>Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário 
+Sistema marca notificação como visualizada
+Sistema deleta a notificação da aba de notificações do usuário</t>
+  </si>
+  <si>
+    <t>Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário
+Apenas uma notificação existe na aba de notificações</t>
+  </si>
+  <si>
+    <t>4. Usuário clica no link da thread existente na notificação enviada</t>
+  </si>
+  <si>
+    <t>5. Sistema exibe a thread da notificação</t>
+  </si>
+  <si>
+    <t>(Necessário ter a thread com subject "Teste3" na lista de threads visualizadas para receber a notificação)
+Realizar a postagem de um comentário na thread "Teste3"
+Realizar a postagem de outro comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação</t>
+  </si>
+  <si>
+    <t>(Necessário ter a thread com subject "Teste3" na lista de threads visualizadas para receber a notificação)
+Realizar a postagem de um comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação
+Clicar no link da thread existente na mensagem da notificação</t>
+  </si>
+  <si>
+    <t>Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário
+Sistema marca a notificação como visualizada
+Sistema abre a thread do link da notificação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário
+Sistema marca a notificação como visualizada
+Sistema envia uma notificação de que houveram postagens novas na thread "Teste3" para o usuário
+Sistema marca a notificação como visualizada
+</t>
+  </si>
+  <si>
+    <t>(Necessário ter a thread com subject "Teste3" na lista de threads visualizadas para receber a notificação)
+Realizar a postagem de um comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação
+Realizar a postagem de outro comentário na thread "Teste3"
+Clicar na área de notificações no cabeçalho para visualizar a notificação</t>
+  </si>
+  <si>
+    <t>1. Administrador localiza a thread com as postagens que deseja deletar</t>
+  </si>
+  <si>
+    <t>2. Administrador seleciona as postagens clicando no ícone Select Post</t>
+  </si>
+  <si>
+    <t>3. Administrador aperta o botão Delete Post localizado no rodapé da thread</t>
+  </si>
+  <si>
+    <t>4. Sistema deleta as mensagens do banco de dados</t>
+  </si>
+  <si>
+    <t>Postagens são deletadas da thread</t>
+  </si>
+  <si>
+    <t>Visualizar thread com subject "TesteX"
+Selecionar a segunda e a terceira postagens da thread, com comentário "Apague isto"
+Clicar no ícone Select Post
+Clicar no botão Delete Post</t>
+  </si>
+  <si>
+    <t>Visualizar thread com subject "TesteX"
+Selecionar a primeira postagem com o comentário "Apague a Thread"
+Clicar no ícone Select Post
+Clicar no botão Delete Post</t>
+  </si>
+  <si>
+    <t>Thread é deletada e o sistema retorna para a janela de visualização de threads da primeira tag da thread apagada</t>
+  </si>
+  <si>
+    <t>1. Administrador localiza alguma postagem do usuário que deseja banir</t>
+  </si>
+  <si>
+    <t>2. Administrador seleciona o ícone Banir Usuário localizado no topo da postagem</t>
+  </si>
+  <si>
+    <t>3. Sistema exibe uma tela para que seja selecionado o tempo de banimento</t>
+  </si>
+  <si>
+    <t>4. Administrador escolhe dentro das seguintes opções: 1 dia; 1 semana; 1 ano; Eternamente</t>
+  </si>
+  <si>
+    <t>5. Administrador clica no botão Confirm</t>
+  </si>
+  <si>
+    <t>6. Sistema bane o usuário pelo IP, inserindo-o na lista de IPs banidos e assim o impedindo de realizar novas postagens dentro do tempo de banimento</t>
+  </si>
+  <si>
+    <t>7. Sistema exibe uma mensagem de banimento no topo da postagem que foi selecionada</t>
+  </si>
+  <si>
+    <t>(Necessário que a primeira postagem da thread "TesteBan" seja de um usuário com IP diferente do administrador)
+Clicar para visualizar a thread "TesteBan"
+Clicar no ícone banir usuário da primeira postagem
+Selecionar o tempo exclusivo para testes de 5 minutos
+Clicar no botão Confirm</t>
+  </si>
+  <si>
+    <t>Sistema abre uma janela para seleção do tempo
+Sistema exibe uma mensagem de sucesso e efetua o banimento do IP do usuário selecionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentar realizar a postagem com comment "TesteTeste" na thread "TesteBan"
+Esperar 5 minutos
+Tentar realizar a postagem com comment "TesteSucesso" na thread "TesteBan"
+</t>
+  </si>
+  <si>
+    <t>Sistema exibe uma mensagem de erro informando que o usuário está banido por 5 desde o timestamp xxxxxx
+Sistema exibe uma mensagem de comentário postado com sucesso
+Thread possui apenas  o comentário "TesteSucesso"</t>
+  </si>
+  <si>
+    <t>Usuário banido por 5 minutos tenta postar</t>
+  </si>
+  <si>
+    <t>(Necessário que a primeira postagem da thread "TesteBan" seja de um usuário com IP diferente do administrador)
+Clicar para visualizar a thread "TesteBan"
+Clicar no ícone banir usuário da primeira postagem
+Clicar no botão Confirm</t>
+  </si>
+  <si>
+    <t>Sistema abre uma janela para seleção do tempo
+Sistema exibe uma mensagem de erro informando que faltou selecionar o tempo do banimento</t>
+  </si>
+  <si>
+    <t>1. Administrador localiza a thread que deseja alterar as tags</t>
+  </si>
+  <si>
+    <t>2. Administrador seleciona o ícone Change Tags localizada na postagem inicial da thread</t>
+  </si>
+  <si>
+    <t>3.Sistema exibe uma área ao lado da postagem com opções de tags para selecionar</t>
+  </si>
+  <si>
+    <t>4. Administrador seleciona as tags que considera adequadas para a determinada thread</t>
+  </si>
+  <si>
+    <t>5. Administrador seleciona o botão Confim</t>
+  </si>
+  <si>
+    <t>6. Sistema altera as tags da postagem inicial para as novas tags escolhidas pelo administrador</t>
+  </si>
+  <si>
+    <t>Sistema exibe thread "TesteTag" que possui a tag Tecnologia
+Sistema exibe área com opções de tags para selecionar
+Tags da thread passam a ser Música e Video Games</t>
+  </si>
+  <si>
+    <t>Clicar para visualização a thread "TesteTag"
+Clicar no ícone Change Tags
+Selecionar as Tags Música e Video Games
+Clicar no botão confirm</t>
+  </si>
+  <si>
+    <t>1. Nova thread é criada em determinada tag</t>
+  </si>
+  <si>
+    <t>2. Sistema fecha a thread no fim da lista de threads de determinada tag, impedindo que ela reapareça na listagem de threads abertas daquela tag</t>
+  </si>
+  <si>
+    <t>Thread no topo da lista de threads arquivadas é a thread com postagem inicial de "TesteArquivaçãoSucesso"</t>
+  </si>
+  <si>
+    <t>(Necessário encher a tag Anime com threads, sendo a última a com postagem inicial de "TesteArquivaçãoSucesso")
+Criar Thread com comentário "TesteArquivação"
+Clicar no ícone abrir lista de threads arquivadas topo da listagem de threads da tag Anime</t>
+  </si>
+  <si>
+    <t>1. Thread permanece no arquivo da última tag ao qual o arquivou por duas semanas</t>
+  </si>
+  <si>
+    <t>2. Sistema deleta a thread do banco de dados</t>
+  </si>
+  <si>
+    <t>1. Administrador localiza a thread que deseja deletar</t>
+  </si>
+  <si>
+    <t>2. Administrador seleciona a postagem inicial da thread clicando no ícone Select Post ao lado da postagem</t>
+  </si>
+  <si>
+    <t>4. Sistema deleta a thread do banco de dados</t>
+  </si>
+  <si>
+    <t>(Para fins de teste, o tempo na lista de threads arquivadas será de 1 minuto)
+(Necessário encher a tag Música com threads, sendo a última a com postagem inicial de "TesteAutoDelete")
+Criar Thread com comentário "Banish that thread to the Shadow Realm!"
+Clicar no ícone abrir lista de threads arquivadas topo da listagem de threads da tag Anime
+Esperar 1 minuto
+Atualizar a página com alista de threads arquivadas</t>
+  </si>
+  <si>
+    <t>Thread no topo da lista de threads arquivadas é a thread com postagem inicial de "TesteAutoDelete"
+Listagem de threads arquivadas após 1 minuto está vazia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1650,6 +1883,12 @@
     <font>
       <u/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1850,7 +2089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1904,6 +2143,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1952,49 +2203,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="104">
     <dxf>
       <font>
         <color rgb="FF7030A0"/>
@@ -2907,11 +3132,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2949,12 +3174,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2977,110 +3202,110 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="36"/>
+      <c r="F11" s="39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3099,26 +3324,26 @@
     <mergeCell ref="F11:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F13">
-    <cfRule type="containsText" dxfId="103" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="97" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="96" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="101" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="94" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="93" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="98" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3131,8 +3356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,11 +3380,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3197,12 +3422,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3225,150 +3450,150 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="A12" s="33">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3387,26 +3612,26 @@
     <mergeCell ref="D12:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F30 F30:F1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3416,10 +3641,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3442,11 +3667,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3471,7 +3696,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F129,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F129,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3484,12 +3709,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3511,105 +3736,242 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>2</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="41"/>
+    </row>
+    <row r="12" spans="1:6" ht="360" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>3</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>4</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="1:6" ht="351.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>5</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="18">
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F9">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F30 F30:F1048576">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,11 +3994,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3661,7 +4023,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F124,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F124,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3674,12 +4036,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3701,92 +4063,149 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>2</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
+    </row>
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="41"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F10 F14:F1048576">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3796,10 +4215,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,11 +4241,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3851,7 +4270,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F131,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F131,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3864,12 +4283,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3891,92 +4310,227 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40"/>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="40"/>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="B21:F21"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="F6:F12"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="D14:D20"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F36 F31:F1048576">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3986,10 +4540,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,11 +4566,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4041,7 +4595,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F122,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F122,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4054,12 +4608,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4081,92 +4635,116 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="F6:F11"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F6 F12:F1048576">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4176,10 +4754,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,11 +4780,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4231,7 +4809,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F118,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F118,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4244,12 +4822,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4271,92 +4849,76 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+    <row r="7" spans="1:6" ht="243" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F7">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4366,10 +4928,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4392,11 +4954,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4421,7 +4983,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>IF(COUNTIF(F6:F121,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F121,"Reprovado")=0,"Aprovado","Reprovado"))</f>
+        <f>IF(COUNTIF(F6:F122,"Não Executado")&gt;0,"Incerto",IF(COUNTIF(F6:F122,"Reprovado")=0,"Aprovado","Reprovado"))</f>
         <v>Incerto</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4434,12 +4996,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4461,92 +5023,129 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="B6" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="7" spans="1:6" ht="351.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>2</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
+    </row>
+    <row r="11" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="41"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Reprovado">
+  <conditionalFormatting sqref="F6:F8">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F8 F12:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4582,11 +5181,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4624,12 +5223,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4652,120 +5251,120 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="36"/>
+      <c r="F11" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -4825,11 +5424,11 @@
       <c r="A19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -4848,34 +5447,34 @@
     <mergeCell ref="F11:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="97" priority="13" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="91" priority="13" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="14" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="90" priority="14" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="11" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="88" priority="11" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="87" priority="12" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F15">
-    <cfRule type="containsText" dxfId="92" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="85" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="90" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4912,11 +5511,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4954,12 +5553,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -4982,120 +5581,120 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="36"/>
+      <c r="F11" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
@@ -5134,86 +5733,75 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="33">
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="35" t="s">
+      <c r="E18" s="36"/>
+      <c r="F18" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="F18:F22"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A10"/>
@@ -5221,28 +5809,39 @@
     <mergeCell ref="D6:D10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F11">
-    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="5" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="80" priority="5" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="6" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="79" priority="6" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F18 F23:F1048576">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5278,11 +5877,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5320,12 +5919,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5348,100 +5947,100 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="A10" s="33">
         <v>2</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="35" t="s">
+      <c r="E10" s="36"/>
+      <c r="F10" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -5465,20 +6064,14 @@
       <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:A9"/>
@@ -5486,28 +6079,34 @@
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="F6:F9"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F10">
-    <cfRule type="containsText" dxfId="83" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F30 F30:F1048576">
-    <cfRule type="cellIs" dxfId="78" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5543,11 +6142,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5585,12 +6184,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5613,62 +6212,62 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
@@ -5692,11 +6291,11 @@
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5710,26 +6309,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F11">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5766,11 +6365,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5808,12 +6407,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -5836,62 +6435,62 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
@@ -5915,11 +6514,11 @@
       <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5933,26 +6532,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F11">
-    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5988,11 +6587,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6030,12 +6629,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -6058,62 +6657,62 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
@@ -6173,11 +6772,11 @@
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6191,26 +6790,26 @@
     <mergeCell ref="F6:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F13">
-    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="59" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="58" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6222,7 +6821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -6246,11 +6845,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6288,12 +6887,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -6316,170 +6915,170 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="33">
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="36"/>
+      <c r="F13" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -6498,26 +7097,26 @@
     <mergeCell ref="D13:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="59" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F30 F30:F1048576">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6553,11 +7152,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6595,12 +7194,12 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -6623,80 +7222,80 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="A6" s="33">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="33">
         <v>2</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="35" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="39" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -6715,26 +7314,26 @@
     <mergeCell ref="F9:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F9">
-    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"Incerto"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Aprovado">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="Aprovado">
       <formula>NOT(ISERROR(SEARCH("Aprovado",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Reprovado">
+    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Reprovado">
       <formula>NOT(ISERROR(SEARCH("Reprovado",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9 F11:F1048576">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"Não executado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>